<commit_message>
did serie b draws and more last man
</commit_message>
<xml_diff>
--- a/last_man_picks.xlsx
+++ b/last_man_picks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexandergreen/Documents/fun/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A27EF2E1-54C1-1E46-9E6A-B5A9BFEBF545}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10797D82-B6A4-6A47-81D3-BE08EE08C333}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15640" yWindow="2860" windowWidth="17260" windowHeight="9260" xr2:uid="{D0919C0E-71B2-7242-9ED6-9308DB0B209C}"/>
+    <workbookView xWindow="4460" yWindow="820" windowWidth="23400" windowHeight="13240" xr2:uid="{D0919C0E-71B2-7242-9ED6-9308DB0B209C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="29">
   <si>
     <t>week</t>
   </si>
@@ -54,10 +54,64 @@
     <t>League Cup Final</t>
   </si>
   <si>
-    <t>city</t>
-  </si>
-  <si>
-    <t>liverpool</t>
+    <t>Arsenal</t>
+  </si>
+  <si>
+    <t>Cardiff City</t>
+  </si>
+  <si>
+    <t>Manchester United</t>
+  </si>
+  <si>
+    <t>Burnley</t>
+  </si>
+  <si>
+    <t>Chelsea</t>
+  </si>
+  <si>
+    <t>Huddersfield Town</t>
+  </si>
+  <si>
+    <t>Southampton</t>
+  </si>
+  <si>
+    <t>Manchester City</t>
+  </si>
+  <si>
+    <t>West Ham United</t>
+  </si>
+  <si>
+    <t>Wolverhampton</t>
+  </si>
+  <si>
+    <t>Leicester City</t>
+  </si>
+  <si>
+    <t>Fulham</t>
+  </si>
+  <si>
+    <t>Crystal Palace</t>
+  </si>
+  <si>
+    <t>Tottenham Hotspur</t>
+  </si>
+  <si>
+    <t>Liverpool</t>
+  </si>
+  <si>
+    <t>Palace</t>
+  </si>
+  <si>
+    <t>Joker</t>
+  </si>
+  <si>
+    <t>Based on biggest draw prob and biggest increase in prob</t>
+  </si>
+  <si>
+    <t>everton</t>
+  </si>
+  <si>
+    <t>watford</t>
   </si>
 </sst>
 </file>
@@ -418,10 +472,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41E3C2C6-C89E-814D-B001-A5E703EAFC18}">
-  <dimension ref="A1:I14"/>
+  <dimension ref="A1:I28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -461,6 +515,15 @@
       <c r="B2" s="1">
         <v>43494</v>
       </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2">
+        <v>0.67679999999999996</v>
+      </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3">
@@ -469,6 +532,15 @@
       <c r="B3" s="1">
         <v>43498</v>
       </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3">
+        <v>0.78599999999999903</v>
+      </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4">
@@ -477,9 +549,15 @@
       <c r="B4" s="2">
         <v>43505</v>
       </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
+      <c r="C4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4">
+        <v>0.55500000000000005</v>
+      </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B5" s="1">
@@ -496,6 +574,15 @@
       <c r="B6" s="1">
         <v>43522</v>
       </c>
+      <c r="C6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6">
+        <v>0.84850000000000003</v>
+      </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7">
@@ -504,9 +591,15 @@
       <c r="B7" s="2">
         <v>43526</v>
       </c>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
+      <c r="C7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7">
+        <v>0.56259999999999999</v>
+      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8">
@@ -515,11 +608,14 @@
       <c r="B8" s="2">
         <v>43533</v>
       </c>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="I8" t="s">
-        <v>9</v>
+      <c r="C8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8">
+        <v>0.55730000000000002</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
@@ -533,9 +629,7 @@
         <v>6</v>
       </c>
       <c r="G9" s="3"/>
-      <c r="I9" s="3" t="s">
-        <v>10</v>
-      </c>
+      <c r="I9" s="3"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10">
@@ -544,9 +638,21 @@
       <c r="B10" s="2">
         <v>43554</v>
       </c>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
+      <c r="C10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10">
+        <v>0.57830000000000004</v>
+      </c>
+      <c r="F10" t="s">
+        <v>25</v>
+      </c>
+      <c r="G10" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B11" s="1">
@@ -565,7 +671,15 @@
       <c r="B12" s="1">
         <v>43568</v>
       </c>
-      <c r="C12" s="3"/>
+      <c r="C12" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" t="s">
+        <v>14</v>
+      </c>
+      <c r="E12">
+        <v>0.80310000000000004</v>
+      </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13">
@@ -574,7 +688,15 @@
       <c r="B13" s="1">
         <v>43575</v>
       </c>
-      <c r="C13" s="3"/>
+      <c r="C13" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E13">
+        <v>0.56610000000000005</v>
+      </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14">
@@ -583,6 +705,55 @@
       <c r="B14" s="1">
         <v>43582</v>
       </c>
+      <c r="C14" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" t="s">
+        <v>14</v>
+      </c>
+      <c r="E14">
+        <v>0.8921</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C15" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C16" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D19" s="1"/>
+    </row>
+    <row r="20" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D20" s="1"/>
+    </row>
+    <row r="21" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D21" s="1"/>
+    </row>
+    <row r="22" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D22" s="1"/>
+    </row>
+    <row r="23" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D23" s="1"/>
+    </row>
+    <row r="24" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D24" s="1"/>
+    </row>
+    <row r="25" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D25" s="1"/>
+    </row>
+    <row r="26" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D26" s="1"/>
+    </row>
+    <row r="27" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D27" s="1"/>
+    </row>
+    <row r="28" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D28" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>